<commit_message>
Fixes to GP02HYPM 1 Cal
https://uframe-cm.ooi.rutgers.edu/issues/3593
</commit_message>
<xml_diff>
--- a/GP02HYPM/Omaha_Cal_Info_GP02HYPM_00001.xlsx
+++ b/GP02HYPM/Omaha_Cal_Info_GP02HYPM_00001.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="12720" windowHeight="12345"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="12720" windowHeight="12345" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -910,6 +910,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -940,10 +1008,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="454545"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="FAFAFA"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1224,7 +1292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
@@ -1355,10 +1423,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="480" activePane="bottomLeft"/>
       <selection activeCell="G1" sqref="G1:K1048576"/>
-      <selection pane="bottomLeft" activeCell="E45" sqref="E45"/>
+      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2044,7 +2112,7 @@
         <v>1</v>
       </c>
       <c r="D34" s="1">
-        <v>10261</v>
+        <v>3710261</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>15</v>
@@ -2064,7 +2132,7 @@
         <v>1</v>
       </c>
       <c r="D35" s="36">
-        <v>10261</v>
+        <v>3710261</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>16</v>
@@ -2084,7 +2152,7 @@
         <v>1</v>
       </c>
       <c r="D36" s="36">
-        <v>10261</v>
+        <v>3710261</v>
       </c>
       <c r="E36" s="35" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Redmine ticket 8587 cal sheets updated for GP02HYPM deployments 1 & 2.
</commit_message>
<xml_diff>
--- a/GP02HYPM/Omaha_Cal_Info_GP02HYPM_00001.xlsx
+++ b/GP02HYPM/Omaha_Cal_Info_GP02HYPM_00001.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gauls\Documents\Project Info\WHOI\Marine Integration - OOI\OOInet Migration\Integration\Cal and Ingest Sheets\Sheets from -test 2015-08-19\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gauls\Documents\Project Info\WHOI\Marine Integration - OOI\OOInet Migration\Integration\Cal and Ingest Sheets\Repaired GIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="48" windowWidth="12720" windowHeight="12348"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14028" windowHeight="4440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="62">
   <si>
     <t>Ref Des</t>
   </si>
@@ -68,9 +68,6 @@
     <t>GP02HYPM-WFP03-05-VEL3DL000</t>
   </si>
   <si>
-    <t>GP02HYPM-RIS01-01-CTDMOG000</t>
-  </si>
-  <si>
     <t>GP02HYPM-00001</t>
   </si>
   <si>
@@ -167,9 +164,6 @@
     <t>GP02HYPM</t>
   </si>
   <si>
-    <t>GP02HYPM-MPC04-01-ZPLSGA000 will be added in later deployments</t>
-  </si>
-  <si>
     <t>Default per &lt;flo_scat_seawater(degC, psu, theta=117.0, wlngth=700.0, delta=0.039)&gt;</t>
   </si>
   <si>
@@ -186,6 +180,177 @@
   </si>
   <si>
     <t>Data End</t>
+  </si>
+  <si>
+    <t>GP02HYPM-MPM01-02-ZPLSGA009 will be added in later deployments</t>
+  </si>
+  <si>
+    <t>GP02HYPM-MPM01-02-ZPLSGA010 will be added in later deployments</t>
+  </si>
+  <si>
+    <r>
+      <t>GP02HYPM-WFP02-00-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WFPENG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>GP02HYPM-WFP03-00-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WFPENG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>GP02HYPM-GP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>01-00-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SIOENG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>000</t>
+    </r>
+  </si>
+  <si>
+    <t>GP02HYPM-00001-GPM01</t>
+  </si>
+  <si>
+    <t>This is a made-up serial number for the controller card</t>
+  </si>
+  <si>
+    <t>It is not clear which of the two WFP serial numbers go with which WFP</t>
+  </si>
+  <si>
+    <r>
+      <t>GP02HYPM-RI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>01-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>02</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-CTDMOG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>061</t>
+    </r>
+  </si>
+  <si>
+    <t>GP02HYPM-RIM01-02-CTDMOG061</t>
+  </si>
+  <si>
+    <t>Nominal imodem ID is 39, but actual for this deployment is 61</t>
   </si>
 </sst>
 </file>
@@ -384,7 +549,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -412,6 +577,12 @@
       <patternFill patternType="solid">
         <fgColor indexed="55"/>
         <bgColor indexed="50"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -624,7 +795,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -762,6 +933,31 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="57" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="57" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1217,7 +1413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
@@ -1236,7 +1432,9 @@
     <col min="11" max="11" width="22.6640625" style="5" customWidth="1"/>
     <col min="12" max="12" width="17.109375" style="5" customWidth="1"/>
     <col min="13" max="13" width="17.88671875" style="5" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="5"/>
+    <col min="14" max="14" width="8.88671875" style="5"/>
+    <col min="15" max="15" width="9.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="9" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
@@ -1244,54 +1442,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="G1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="8" t="s">
-        <v>32</v>
-      </c>
       <c r="L1" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="M1" s="33" t="s">
+      <c r="O1" s="33" t="s">
         <v>50</v>
-      </c>
-      <c r="N1" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="O1" s="33" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
@@ -1306,16 +1504,16 @@
         <v>41842</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="32">
@@ -1346,23 +1544,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="480" activePane="bottomLeft"/>
-      <selection activeCell="E1" sqref="E1:F1048576"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="33.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="84.44140625" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="11" width="10.6640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="8.88671875" style="1"/>
@@ -1376,7 +1572,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>2</v>
@@ -1388,7 +1584,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -1405,7 +1601,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="10">
         <v>1</v>
@@ -1414,13 +1610,13 @@
         <v>2736</v>
       </c>
       <c r="E3" s="34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="34">
         <v>51</v>
       </c>
       <c r="G3" s="45" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1428,7 +1624,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="10">
         <v>1</v>
@@ -1437,7 +1633,7 @@
         <v>2736</v>
       </c>
       <c r="E4" s="34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="34">
         <v>1.871E-6</v>
@@ -1449,7 +1645,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="10">
         <v>1</v>
@@ -1458,7 +1654,7 @@
         <v>2736</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="46">
         <v>52</v>
@@ -1470,7 +1666,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="10">
         <v>1</v>
@@ -1479,7 +1675,7 @@
         <v>2736</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="46">
         <v>7.3000000000000001E-3</v>
@@ -1491,7 +1687,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="10">
         <v>1</v>
@@ -1500,13 +1696,13 @@
         <v>2736</v>
       </c>
       <c r="E7" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="46">
-        <v>117</v>
+        <v>37</v>
+      </c>
+      <c r="F7" s="49">
+        <v>140</v>
       </c>
       <c r="G7" s="44" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1514,7 +1710,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="10">
         <v>1</v>
@@ -1523,13 +1719,13 @@
         <v>2736</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F8" s="46">
         <v>700</v>
       </c>
       <c r="G8" s="44" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1537,7 +1733,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="10">
         <v>1</v>
@@ -1546,13 +1742,13 @@
         <v>2736</v>
       </c>
       <c r="E9" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="46">
-        <v>1.08</v>
+        <v>39</v>
+      </c>
+      <c r="F9" s="49">
+        <v>1.1299999999999999</v>
       </c>
       <c r="G9" s="44" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1560,7 +1756,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="10">
         <v>1</v>
@@ -1569,13 +1765,13 @@
         <v>2736</v>
       </c>
       <c r="E10" s="46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" s="45">
         <v>3.9E-2</v>
       </c>
       <c r="G10" s="44" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1589,7 +1785,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="10">
         <v>1</v>
@@ -1598,13 +1794,13 @@
         <v>1086</v>
       </c>
       <c r="E12" s="42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F12" s="43">
         <v>50.070666666666668</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1612,7 +1808,7 @@
         <v>6</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="10">
         <v>1</v>
@@ -1621,222 +1817,162 @@
         <v>1086</v>
       </c>
       <c r="E13" s="42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" s="43">
         <v>-144.798</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="37"/>
+      <c r="B14" s="36"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="43"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="10">
-        <v>1</v>
-      </c>
-      <c r="D14" s="4">
+      <c r="B15" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="10">
+        <v>1</v>
+      </c>
+      <c r="D15" s="4">
         <v>107</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="E15" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="43">
+        <v>50.070666666666668</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="10">
+        <v>1</v>
+      </c>
+      <c r="D16" s="30">
+        <v>107</v>
+      </c>
+      <c r="E16" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="43">
-        <v>50.070666666666668</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="10">
-        <v>1</v>
-      </c>
-      <c r="D15" s="30">
-        <v>107</v>
-      </c>
-      <c r="E15" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="43">
+      <c r="F16" s="43">
         <v>-144.798</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="10">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4">
-        <v>1024</v>
-      </c>
-      <c r="E16" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="43">
-        <v>50.070666666666668</v>
-      </c>
-    </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="36">
-        <v>1</v>
-      </c>
-      <c r="D17" s="30">
-        <v>1024</v>
-      </c>
-      <c r="E17" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="43">
-        <v>-144.798</v>
-      </c>
+      <c r="A17" s="37"/>
+      <c r="B17" s="36"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="43"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="10">
         <v>1</v>
       </c>
       <c r="D18" s="4">
-        <v>2350</v>
-      </c>
-      <c r="E18" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="34">
-        <v>48</v>
-      </c>
-      <c r="G18" s="45" t="s">
-        <v>35</v>
+        <v>1024</v>
+      </c>
+      <c r="E18" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="43">
+        <v>50.070666666666668</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="36">
+        <v>1</v>
+      </c>
+      <c r="D19" s="30">
+        <v>1024</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="43">
+        <v>-144.798</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="37"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="43"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="53">
+        <v>1</v>
+      </c>
+      <c r="D21" s="50">
+        <v>12936</v>
+      </c>
+      <c r="E21" s="42"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="37"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="43"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="10">
-        <v>1</v>
-      </c>
-      <c r="D19" s="30">
+      <c r="B23" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="10">
+        <v>1</v>
+      </c>
+      <c r="D23" s="4">
         <v>2350</v>
       </c>
-      <c r="E19" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" s="34">
-        <v>2.0339999999999999E-6</v>
-      </c>
-      <c r="G19" s="42"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="10">
-        <v>1</v>
-      </c>
-      <c r="D20" s="30">
-        <v>2350</v>
-      </c>
-      <c r="E20" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="46">
+      <c r="E23" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="34">
         <v>48</v>
       </c>
-      <c r="G20" s="45"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="10">
-        <v>1</v>
-      </c>
-      <c r="D21" s="30">
-        <v>2350</v>
-      </c>
-      <c r="E21" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" s="46">
-        <v>7.3000000000000001E-3</v>
-      </c>
-      <c r="G21" s="45"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="10">
-        <v>1</v>
-      </c>
-      <c r="D22" s="30">
-        <v>2350</v>
-      </c>
-      <c r="E22" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" s="46">
-        <v>117</v>
-      </c>
-      <c r="G22" s="44" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="10">
-        <v>1</v>
-      </c>
-      <c r="D23" s="30">
-        <v>2350</v>
-      </c>
-      <c r="E23" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="F23" s="46">
-        <v>700</v>
-      </c>
-      <c r="G23" s="44" t="s">
-        <v>48</v>
+      <c r="G23" s="45" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1844,7 +1980,7 @@
         <v>9</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C24" s="10">
         <v>1</v>
@@ -1852,22 +1988,20 @@
       <c r="D24" s="30">
         <v>2350</v>
       </c>
-      <c r="E24" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="F24" s="46">
-        <v>1.08</v>
-      </c>
-      <c r="G24" s="44" t="s">
-        <v>48</v>
-      </c>
+      <c r="E24" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="34">
+        <v>2.0339999999999999E-6</v>
+      </c>
+      <c r="G24" s="42"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="37" t="s">
         <v>9</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25" s="10">
         <v>1</v>
@@ -1876,214 +2010,431 @@
         <v>2350</v>
       </c>
       <c r="E25" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="F25" s="45">
-        <v>3.9E-2</v>
-      </c>
-      <c r="G25" s="44" t="s">
-        <v>47</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F25" s="46">
+        <v>48</v>
+      </c>
+      <c r="G25" s="45"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="37"/>
-      <c r="B26" s="36"/>
-      <c r="D26" s="30"/>
-      <c r="G26" s="44"/>
+      <c r="A26" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="10">
+        <v>1</v>
+      </c>
+      <c r="D26" s="30">
+        <v>2350</v>
+      </c>
+      <c r="E26" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" s="46">
+        <v>7.3000000000000001E-3</v>
+      </c>
+      <c r="G26" s="45"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>14</v>
+      <c r="A27" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="36" t="s">
+        <v>13</v>
       </c>
       <c r="C27" s="10">
         <v>1</v>
       </c>
-      <c r="D27" s="4">
-        <v>1106</v>
-      </c>
-      <c r="E27" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="41">
-        <v>50.070666666666668</v>
+      <c r="D27" s="30">
+        <v>2350</v>
+      </c>
+      <c r="E27" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="49">
+        <v>140</v>
+      </c>
+      <c r="G27" s="44" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C28" s="10">
         <v>1</v>
       </c>
       <c r="D28" s="30">
-        <v>1106</v>
-      </c>
-      <c r="E28" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="41">
-        <v>-144.798</v>
+        <v>2350</v>
+      </c>
+      <c r="E28" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" s="46">
+        <v>700</v>
+      </c>
+      <c r="G28" s="44" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>14</v>
+      <c r="A29" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="36" t="s">
+        <v>13</v>
       </c>
       <c r="C29" s="10">
         <v>1</v>
       </c>
-      <c r="D29" s="4">
-        <v>97</v>
-      </c>
-      <c r="E29" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="F29" s="43">
-        <v>50.070666666666668</v>
+      <c r="D29" s="30">
+        <v>2350</v>
+      </c>
+      <c r="E29" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" s="49">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="G29" s="44" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="10">
+        <v>1</v>
+      </c>
+      <c r="D30" s="30">
+        <v>2350</v>
+      </c>
+      <c r="E30" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="45">
+        <v>3.9E-2</v>
+      </c>
+      <c r="G30" s="44" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="37"/>
+      <c r="B31" s="36"/>
+      <c r="D31" s="30"/>
+      <c r="G31" s="44"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="10">
+        <v>1</v>
+      </c>
+      <c r="D32" s="4">
+        <v>1106</v>
+      </c>
+      <c r="E32" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="41">
+        <v>50.070666666666668</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="10">
+        <v>1</v>
+      </c>
+      <c r="D33" s="30">
+        <v>1106</v>
+      </c>
+      <c r="E33" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="41">
+        <v>-144.798</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="37"/>
+      <c r="B34" s="36"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="41"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="10">
-        <v>1</v>
-      </c>
-      <c r="D30" s="30">
+      <c r="B35" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="10">
+        <v>1</v>
+      </c>
+      <c r="D35" s="4">
         <v>97</v>
       </c>
-      <c r="E30" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="F30" s="43">
-        <v>-144.798</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="10">
-        <v>1</v>
-      </c>
-      <c r="D31" s="4">
-        <v>1025</v>
-      </c>
-      <c r="E31" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" s="41">
-        <v>50.070666666666668</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="36">
-        <v>1</v>
-      </c>
-      <c r="D32" s="30">
-        <v>1025</v>
-      </c>
-      <c r="E32" s="42" t="s">
+      <c r="E35" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="F32" s="41">
-        <v>-144.798</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="37"/>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="H33" s="39"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="39"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" s="10">
-        <v>1</v>
-      </c>
-      <c r="D34" s="1">
-        <v>3710261</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F34" s="34">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" s="10">
-        <v>1</v>
-      </c>
-      <c r="D35" s="36">
-        <v>3710261</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F35" s="34">
+      <c r="F35" s="43">
         <v>50.070666666666668</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="37" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B36" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="10">
+        <v>1</v>
+      </c>
+      <c r="D36" s="30">
+        <v>97</v>
+      </c>
+      <c r="E36" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="43">
+        <v>-144.798</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="37"/>
+      <c r="B37" s="36"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="43"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="10">
+        <v>1</v>
+      </c>
+      <c r="D38" s="4">
+        <v>1025</v>
+      </c>
+      <c r="E38" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="41">
+        <v>50.070666666666703</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="36">
+        <v>1</v>
+      </c>
+      <c r="D39" s="30">
+        <v>1025</v>
+      </c>
+      <c r="E39" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="41">
+        <v>-144.798</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="48"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="41"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="53">
+        <v>1</v>
+      </c>
+      <c r="D41" s="50">
+        <v>12774</v>
+      </c>
+      <c r="E41" s="42"/>
+      <c r="F41" s="41"/>
+      <c r="G41" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="H41" s="39"/>
+      <c r="I41" s="39"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="39"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="37"/>
+      <c r="B42" s="36"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="41"/>
+      <c r="G42" s="40"/>
+      <c r="H42" s="39"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
+      <c r="K42" s="39"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="37"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="41"/>
+      <c r="G43" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="H43" s="39"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="39"/>
+      <c r="K43" s="39"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" s="48"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="41"/>
+      <c r="G44" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="H44" s="39"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="39"/>
+      <c r="K44" s="39"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" s="48"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="42"/>
+      <c r="F45" s="41"/>
+      <c r="G45" s="47"/>
+      <c r="H45" s="39"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
+      <c r="K45" s="39"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="10">
+        <v>1</v>
+      </c>
+      <c r="D46" s="1">
+        <v>3710261</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="10">
-        <v>1</v>
-      </c>
-      <c r="D36" s="36">
+      <c r="F46" s="55">
+        <v>1450</v>
+      </c>
+      <c r="G46" s="39" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" s="10">
+        <v>1</v>
+      </c>
+      <c r="D47" s="36">
         <v>3710261</v>
       </c>
-      <c r="E36" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="F36" s="34">
+      <c r="E47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" s="34">
+        <v>50.070666666666668</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B48" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="10">
+        <v>1</v>
+      </c>
+      <c r="D48" s="36">
+        <v>3710261</v>
+      </c>
+      <c r="E48" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" s="34">
         <v>-144.798</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="53">
+        <v>1</v>
+      </c>
+      <c r="D50" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="G50" s="39" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
redmine #9176 cal sheets for GP02HYPM deployements 1-3 changed/added.
</commit_message>
<xml_diff>
--- a/GP02HYPM/Omaha_Cal_Info_GP02HYPM_00001.xlsx
+++ b/GP02HYPM/Omaha_Cal_Info_GP02HYPM_00001.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14025" windowHeight="4440" activeTab="1"/>
+    <workbookView xWindow="6460" yWindow="5940" windowWidth="29600" windowHeight="14420"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -17,12 +17,17 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="64">
   <si>
     <t>Ref Des</t>
   </si>
@@ -118,9 +123,6 @@
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>Melville 130</t>
   </si>
   <si>
     <t>Needs PRESWAT, TEMPWAT, and PRACSAL from nearest CTD</t>
@@ -279,9 +281,6 @@
   </si>
   <si>
     <t>This is a made-up serial number for the controller card</t>
-  </si>
-  <si>
-    <t>It is not clear which of the two WFP serial numbers go with which WFP</t>
   </si>
   <si>
     <r>
@@ -344,19 +343,56 @@
   <si>
     <t>Nominal imodem ID is 39, but actual for this deployment is 61</t>
   </si>
+  <si>
+    <t>MV-130</t>
+  </si>
+  <si>
+    <t>GP02HYPM-MPM01-02-ZPLSGA009</t>
+  </si>
+  <si>
+    <t>GP02HYPM-MPM01-02-ZPLSGA010</t>
+  </si>
+  <si>
+    <r>
+      <t>12936</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-02</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>12774</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-01</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="166" formatCode="h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="168" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -539,6 +575,12 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -614,16 +656,16 @@
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -642,14 +684,14 @@
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -717,14 +759,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -787,7 +829,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -819,10 +861,10 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="16" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -840,10 +882,10 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="16" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -867,13 +909,7 @@
     <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="27" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="27" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -951,6 +987,30 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="27" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="27" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" xfId="57" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="29" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="131">
@@ -1100,7 +1160,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Read Me"/>
@@ -1405,31 +1465,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="19" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="5" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" style="5" customWidth="1"/>
-    <col min="12" max="12" width="17.140625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" style="5" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="5"/>
-    <col min="15" max="15" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.85546875" style="5"/>
+    <col min="1" max="1" width="16.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="19" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="13.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.6640625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="17.1640625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="17.83203125" style="5" customWidth="1"/>
+    <col min="14" max="14" width="8.83203125" style="5"/>
+    <col min="15" max="15" width="9.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="9" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="9" customFormat="1" ht="28">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1437,7 +1495,7 @@
         <v>23</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>24</v>
@@ -1463,74 +1521,81 @@
       <c r="K1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="L1" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="33" t="s">
+      <c r="N1" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="33" t="s">
+      <c r="O1" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:15" s="20" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-      <c r="D2" s="28">
+      <c r="C2" s="54">
+        <v>1</v>
+      </c>
+      <c r="D2" s="55">
         <v>41481</v>
       </c>
-      <c r="E2" s="29">
+      <c r="E2" s="56">
         <v>0.34097222222222223</v>
       </c>
-      <c r="F2" s="28">
+      <c r="F2" s="55">
         <v>41842</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="3">
+      <c r="H2" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="54">
         <v>4219</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="32">
+      <c r="J2" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" s="61">
+        <v>41804</v>
+      </c>
+      <c r="L2" s="30">
         <f>((LEFT(G2,(FIND("°",G2,1)-1)))+(MID(G2,(FIND("°",G2,1)+1),(FIND("'",G2,1))-(FIND("°",G2,1)+1))/60))*(IF(RIGHT(G2,1)="N",1,-1))</f>
         <v>50.070666666666668</v>
       </c>
-      <c r="M2" s="32">
+      <c r="M2" s="30">
         <f>((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="E",1,-1))</f>
         <v>-144.798</v>
       </c>
-      <c r="N2" s="31">
+      <c r="N2" s="29">
         <v>41451</v>
       </c>
-      <c r="O2" s="31">
+      <c r="O2" s="29">
         <v>41593</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="20" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" s="20" customFormat="1">
       <c r="D3" s="26"/>
       <c r="E3" s="27"/>
       <c r="F3" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1538,25 +1603,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="33.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="84.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="10.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="33.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="84.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="10.6640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.85546875" style="1"/>
+    <col min="13" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="16" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="16" customFormat="1">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1564,7 +1632,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>2</v>
@@ -1579,7 +1647,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="16" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="16" customFormat="1">
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
       <c r="C2" s="25"/>
@@ -1588,8 +1656,8 @@
       <c r="F2" s="15"/>
       <c r="G2" s="17"/>
     </row>
-    <row r="3" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" s="36" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -1601,179 +1669,179 @@
       <c r="D3" s="4">
         <v>2736</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="34">
+      <c r="F3" s="32">
         <v>51</v>
       </c>
-      <c r="G3" s="45" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A4" s="37" t="s">
+      <c r="G3" s="43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="10">
         <v>1</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="28">
         <v>2736</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="34">
+      <c r="F4" s="32">
         <v>1.871E-6</v>
       </c>
-      <c r="G4" s="45"/>
-    </row>
-    <row r="5" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A5" s="37" t="s">
+      <c r="G4" s="43"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="10">
         <v>1</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="28">
         <v>2736</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="46">
+      <c r="F5" s="44">
         <v>52</v>
       </c>
-      <c r="G5" s="45"/>
-    </row>
-    <row r="6" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A6" s="37" t="s">
+      <c r="G5" s="43"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="10">
         <v>1</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="28">
         <v>2736</v>
       </c>
-      <c r="E6" s="46" t="s">
+      <c r="E6" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="46">
+      <c r="F6" s="44">
         <v>7.3000000000000001E-3</v>
       </c>
-      <c r="G6" s="45"/>
-    </row>
-    <row r="7" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A7" s="37" t="s">
+      <c r="G6" s="43"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="10">
         <v>1</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="28">
         <v>2736</v>
       </c>
-      <c r="E7" s="46" t="s">
+      <c r="E7" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="47">
+        <v>140</v>
+      </c>
+      <c r="G7" s="42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="10">
+        <v>1</v>
+      </c>
+      <c r="D8" s="28">
+        <v>2736</v>
+      </c>
+      <c r="E8" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="49">
-        <v>140</v>
-      </c>
-      <c r="G7" s="44" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A8" s="37" t="s">
+      <c r="F8" s="44">
+        <v>700</v>
+      </c>
+      <c r="G8" s="42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="10">
-        <v>1</v>
-      </c>
-      <c r="D8" s="30">
+      <c r="B9" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="10">
+        <v>1</v>
+      </c>
+      <c r="D9" s="28">
         <v>2736</v>
       </c>
-      <c r="E8" s="46" t="s">
+      <c r="E9" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="46">
-        <v>700</v>
-      </c>
-      <c r="G8" s="44" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A9" s="37" t="s">
+      <c r="F9" s="59">
+        <v>1.0960000000000001</v>
+      </c>
+      <c r="G9" s="42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="10">
-        <v>1</v>
-      </c>
-      <c r="D9" s="30">
+      <c r="B10" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="28">
         <v>2736</v>
       </c>
-      <c r="E9" s="46" t="s">
+      <c r="E10" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="49">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="G9" s="44" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A10" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="30">
-        <v>2736</v>
-      </c>
-      <c r="E10" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="45">
+      <c r="F10" s="43">
         <v>3.9E-2</v>
       </c>
-      <c r="G10" s="44" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A11" s="37"/>
-      <c r="B11" s="36"/>
-      <c r="D11" s="30"/>
-      <c r="G11" s="44"/>
-    </row>
-    <row r="12" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A12" s="38" t="s">
+      <c r="G10" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="35"/>
+      <c r="B11" s="34"/>
+      <c r="D11" s="28"/>
+      <c r="G11" s="42"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="36" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -1785,45 +1853,45 @@
       <c r="D12" s="4">
         <v>1086</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="E12" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="43">
+      <c r="F12" s="41">
         <v>50.070666666666668</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A13" s="37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="10">
         <v>1</v>
       </c>
-      <c r="D13" s="30">
+      <c r="D13" s="28">
         <v>1086</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="43">
+      <c r="F13" s="41">
         <v>-144.798</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A14" s="37"/>
-      <c r="B14" s="36"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="43"/>
-    </row>
-    <row r="15" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A15" s="38" t="s">
+    <row r="14" spans="1:7">
+      <c r="A14" s="35"/>
+      <c r="B14" s="34"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="41"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="36" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="10" t="s">
@@ -1835,42 +1903,42 @@
       <c r="D15" s="4">
         <v>107</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="43">
+      <c r="F15" s="41">
         <v>50.070666666666668</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A16" s="37" t="s">
+    <row r="16" spans="1:7">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="10">
         <v>1</v>
       </c>
-      <c r="D16" s="30">
+      <c r="D16" s="28">
         <v>107</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="E16" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="43">
+      <c r="F16" s="41">
         <v>-144.798</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A17" s="37"/>
-      <c r="B17" s="36"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="43"/>
-    </row>
-    <row r="18" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A18" s="38" t="s">
+    <row r="17" spans="1:7">
+      <c r="A17" s="35"/>
+      <c r="B17" s="34"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="41"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="36" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="10" t="s">
@@ -1882,70 +1950,68 @@
       <c r="D18" s="4">
         <v>1024</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="43">
+      <c r="F18" s="41">
         <v>50.070666666666668</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A19" s="37" t="s">
+    <row r="19" spans="1:7">
+      <c r="A19" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="36">
-        <v>1</v>
-      </c>
-      <c r="D19" s="30">
+      <c r="B19" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="34">
+        <v>1</v>
+      </c>
+      <c r="D19" s="28">
         <v>1024</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="E19" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="43">
+      <c r="F19" s="41">
         <v>-144.798</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A20" s="37"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="43"/>
-    </row>
-    <row r="21" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A21" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="52" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="53">
-        <v>1</v>
-      </c>
-      <c r="D21" s="50">
-        <v>12936</v>
-      </c>
-      <c r="E21" s="42"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A22" s="37"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="43"/>
-    </row>
-    <row r="23" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A23" s="38" t="s">
+    <row r="20" spans="1:7">
+      <c r="A20" s="35"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="41"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="51">
+        <v>1</v>
+      </c>
+      <c r="D21" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="40"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="37"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="35"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="41"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="36" t="s">
         <v>9</v>
       </c>
       <c r="B23" s="10" t="s">
@@ -1957,179 +2023,179 @@
       <c r="D23" s="4">
         <v>2350</v>
       </c>
-      <c r="E23" s="34" t="s">
+      <c r="E23" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="34">
+      <c r="F23" s="32">
         <v>48</v>
       </c>
-      <c r="G23" s="45" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A24" s="37" t="s">
+      <c r="G23" s="43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="10">
         <v>1</v>
       </c>
-      <c r="D24" s="30">
+      <c r="D24" s="28">
         <v>2350</v>
       </c>
-      <c r="E24" s="34" t="s">
+      <c r="E24" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="F24" s="34">
+      <c r="F24" s="32">
         <v>2.0339999999999999E-6</v>
       </c>
-      <c r="G24" s="42"/>
-    </row>
-    <row r="25" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A25" s="37" t="s">
+      <c r="G24" s="40"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="10">
         <v>1</v>
       </c>
-      <c r="D25" s="30">
+      <c r="D25" s="28">
         <v>2350</v>
       </c>
-      <c r="E25" s="46" t="s">
+      <c r="E25" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="F25" s="46">
+      <c r="F25" s="44">
         <v>48</v>
       </c>
-      <c r="G25" s="45"/>
-    </row>
-    <row r="26" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A26" s="37" t="s">
+      <c r="G25" s="43"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="10">
         <v>1</v>
       </c>
-      <c r="D26" s="30">
+      <c r="D26" s="28">
         <v>2350</v>
       </c>
-      <c r="E26" s="46" t="s">
+      <c r="E26" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="F26" s="46">
+      <c r="F26" s="44">
         <v>7.3000000000000001E-3</v>
       </c>
-      <c r="G26" s="45"/>
-    </row>
-    <row r="27" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A27" s="37" t="s">
+      <c r="G26" s="43"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C27" s="10">
         <v>1</v>
       </c>
-      <c r="D27" s="30">
+      <c r="D27" s="28">
         <v>2350</v>
       </c>
-      <c r="E27" s="46" t="s">
+      <c r="E27" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="47">
+        <v>140</v>
+      </c>
+      <c r="G27" s="42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="10">
+        <v>1</v>
+      </c>
+      <c r="D28" s="28">
+        <v>2350</v>
+      </c>
+      <c r="E28" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="49">
-        <v>140</v>
-      </c>
-      <c r="G27" s="44" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A28" s="37" t="s">
+      <c r="F28" s="44">
+        <v>700</v>
+      </c>
+      <c r="G28" s="42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="10">
-        <v>1</v>
-      </c>
-      <c r="D28" s="30">
+      <c r="B29" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="10">
+        <v>1</v>
+      </c>
+      <c r="D29" s="28">
         <v>2350</v>
       </c>
-      <c r="E28" s="46" t="s">
+      <c r="E29" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="46">
-        <v>700</v>
-      </c>
-      <c r="G28" s="44" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A29" s="37" t="s">
+      <c r="F29" s="59">
+        <v>1.0960000000000001</v>
+      </c>
+      <c r="G29" s="42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" s="10">
-        <v>1</v>
-      </c>
-      <c r="D29" s="30">
+      <c r="B30" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="10">
+        <v>1</v>
+      </c>
+      <c r="D30" s="28">
         <v>2350</v>
       </c>
-      <c r="E29" s="46" t="s">
+      <c r="E30" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="F29" s="49">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="G29" s="44" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A30" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="10">
-        <v>1</v>
-      </c>
-      <c r="D30" s="30">
-        <v>2350</v>
-      </c>
-      <c r="E30" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="F30" s="45">
+      <c r="F30" s="43">
         <v>3.9E-2</v>
       </c>
-      <c r="G30" s="44" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A31" s="37"/>
-      <c r="B31" s="36"/>
-      <c r="D31" s="30"/>
-      <c r="G31" s="44"/>
-    </row>
-    <row r="32" spans="1:7" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A32" s="38" t="s">
+      <c r="G30" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="35"/>
+      <c r="B31" s="34"/>
+      <c r="D31" s="28"/>
+      <c r="G31" s="42"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="36" t="s">
         <v>10</v>
       </c>
       <c r="B32" s="10" t="s">
@@ -2141,42 +2207,42 @@
       <c r="D32" s="4">
         <v>1106</v>
       </c>
-      <c r="E32" s="42" t="s">
+      <c r="E32" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="F32" s="41">
+      <c r="F32" s="39">
         <v>50.070666666666668</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A33" s="37" t="s">
+    <row r="33" spans="1:11">
+      <c r="A33" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C33" s="10">
         <v>1</v>
       </c>
-      <c r="D33" s="30">
+      <c r="D33" s="28">
         <v>1106</v>
       </c>
-      <c r="E33" s="42" t="s">
+      <c r="E33" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="F33" s="41">
+      <c r="F33" s="39">
         <v>-144.798</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A34" s="37"/>
-      <c r="B34" s="36"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="41"/>
-    </row>
-    <row r="35" spans="1:11" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A35" s="38" t="s">
+    <row r="34" spans="1:11">
+      <c r="A34" s="35"/>
+      <c r="B34" s="34"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="39"/>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="36" t="s">
         <v>11</v>
       </c>
       <c r="B35" s="10" t="s">
@@ -2188,42 +2254,42 @@
       <c r="D35" s="4">
         <v>97</v>
       </c>
-      <c r="E35" s="34" t="s">
+      <c r="E35" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="F35" s="43">
+      <c r="F35" s="41">
         <v>50.070666666666668</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A36" s="37" t="s">
+    <row r="36" spans="1:11">
+      <c r="A36" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="10">
         <v>1</v>
       </c>
-      <c r="D36" s="30">
+      <c r="D36" s="28">
         <v>97</v>
       </c>
-      <c r="E36" s="34" t="s">
+      <c r="E36" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="F36" s="43">
+      <c r="F36" s="41">
         <v>-144.798</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="37"/>
-      <c r="B37" s="36"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="43"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="38" t="s">
+    <row r="37" spans="1:11">
+      <c r="A37" s="35"/>
+      <c r="B37" s="34"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="41"/>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="36" t="s">
         <v>12</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -2235,123 +2301,125 @@
       <c r="D38" s="4">
         <v>1025</v>
       </c>
-      <c r="E38" s="42" t="s">
+      <c r="E38" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="F38" s="41">
+      <c r="F38" s="39">
         <v>50.070666666666703</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="37" t="s">
+    <row r="39" spans="1:11">
+      <c r="A39" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" s="36">
-        <v>1</v>
-      </c>
-      <c r="D39" s="30">
+      <c r="B39" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="34">
+        <v>1</v>
+      </c>
+      <c r="D39" s="28">
         <v>1025</v>
       </c>
-      <c r="E39" s="42" t="s">
+      <c r="E39" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="F39" s="41">
+      <c r="F39" s="39">
         <v>-144.798</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="48"/>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="42"/>
-      <c r="F40" s="41"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" s="52" t="s">
-        <v>13</v>
-      </c>
-      <c r="C41" s="53">
-        <v>1</v>
-      </c>
-      <c r="D41" s="50">
-        <v>12774</v>
-      </c>
-      <c r="E41" s="42"/>
-      <c r="F41" s="41"/>
-      <c r="G41" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="H41" s="39"/>
-      <c r="I41" s="39"/>
-      <c r="J41" s="39"/>
-      <c r="K41" s="39"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="37"/>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="30"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="41"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
-      <c r="K42" s="39"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="37"/>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="41"/>
-      <c r="G43" s="40" t="s">
+    <row r="40" spans="1:11">
+      <c r="A40" s="46"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="39"/>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="51">
+        <v>1</v>
+      </c>
+      <c r="D41" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="E41" s="40"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="37"/>
+      <c r="K41" s="37"/>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="35"/>
+      <c r="B42" s="34"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="37"/>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" s="34"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="40"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="H43" s="37"/>
+      <c r="I43" s="37"/>
+      <c r="J43" s="37"/>
+      <c r="K43" s="37"/>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" s="34"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="H43" s="39"/>
-      <c r="I43" s="39"/>
-      <c r="J43" s="39"/>
-      <c r="K43" s="39"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="48"/>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="41"/>
-      <c r="G44" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="H44" s="39"/>
-      <c r="I44" s="39"/>
-      <c r="J44" s="39"/>
-      <c r="K44" s="39"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="48"/>
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="42"/>
-      <c r="F45" s="41"/>
-      <c r="G45" s="47"/>
-      <c r="H45" s="39"/>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
-      <c r="K45" s="39"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" s="51" t="s">
-        <v>58</v>
+      <c r="H44" s="37"/>
+      <c r="I44" s="37"/>
+      <c r="J44" s="37"/>
+      <c r="K44" s="37"/>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="46"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="37"/>
+      <c r="K45" s="37"/>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="49" t="s">
+        <v>56</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>13</v>
@@ -2359,78 +2427,83 @@
       <c r="C46" s="10">
         <v>1</v>
       </c>
-      <c r="D46" s="1">
-        <v>3710261</v>
+      <c r="D46" s="60">
+        <v>10261</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F46" s="55">
+      <c r="F46" s="53">
         <v>1450</v>
       </c>
-      <c r="G46" s="39" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="B47" s="36" t="s">
+      <c r="G46" s="37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="14.5" customHeight="1">
+      <c r="A47" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B47" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C47" s="10">
         <v>1</v>
       </c>
-      <c r="D47" s="36">
-        <v>3710261</v>
+      <c r="D47" s="60">
+        <v>10261</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F47" s="34">
+      <c r="F47" s="32">
         <v>50.070666666666668</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="B48" s="36" t="s">
+    <row r="48" spans="1:11" ht="14.5" customHeight="1">
+      <c r="A48" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C48" s="10">
         <v>1</v>
       </c>
-      <c r="D48" s="36">
-        <v>3710261</v>
-      </c>
-      <c r="E48" s="35" t="s">
+      <c r="D48" s="60">
+        <v>10261</v>
+      </c>
+      <c r="E48" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="F48" s="34">
+      <c r="F48" s="32">
         <v>-144.798</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="51" t="s">
+    <row r="50" spans="1:7">
+      <c r="A50" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="51">
+        <v>1</v>
+      </c>
+      <c r="D50" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="B50" s="52" t="s">
-        <v>13</v>
-      </c>
-      <c r="C50" s="53">
-        <v>1</v>
-      </c>
-      <c r="D50" s="54" t="s">
+      <c r="G50" s="37" t="s">
         <v>55</v>
-      </c>
-      <c r="G50" s="39" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>